<commit_message>
Incrementando carrosel no index
</commit_message>
<xml_diff>
--- a/backlogEnviroSense/backlog-EnviroSense.xlsx
+++ b/backlogEnviroSense/backlog-EnviroSense.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Bruno\Sptech\PI\EnviroSense\Enviro-Sense\backlogEnviroSense\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F4BB94-ED12-48F9-8096-ECFBBD03E0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sprint2 Backlog" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sprint3 Backlog" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint2 Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint3 Backlog" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,302 +29,299 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="96">
   <si>
-    <t xml:space="preserve">Projeto EnviroSense - Backlog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requisitos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Descrição</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classificação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplicação WEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela Inicial, Tela de Login, Tela de Cadastro, Tela de Recuperação de Senha, Simulador Financeiro, Sobre Nós, Dashboard.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Essencial.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela Inicial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Título do Projeto, Descrição Sobre o Projeto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela de Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campo de Usuário/E-mail, Campo de Senha, Botão de Visualizar Senha, Botão de Recuperação de Senha, Botão de Login, Botão de Cadastro.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela de Cadastro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campo de Usuário, Campo de E-mail, Campo de Senha, Campo de Confirmar Senha, Botão de Visualizar Senhas, Botão de Confirmar Cadastro.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela de Recuperação de Senha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Campo de E-mail, Botão de Recuperar Senha, Campo de Confirmação de Código.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulador Financeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aplicação para simular o risco de perdas e multas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Importante.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site Institucional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informações Sobre a Solução, Informações Sobre os Desenvolvedores, Informações Sobre o Segmento.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estatísticas, Gráficos, Projeções do dados captados.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documentação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contexto, Objetivo, Justificativa, Escopo, Premissas / Restrições, Requisitos, Diagrama de Visão de Negócio, Protótipo da Aplicação WEB, Projeto Configurado no GitHub.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contexto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Explicação do Problema, Explicação do Mercado, Explicação da Solução.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objetivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pontos a Serem Alcançados.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justificativa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dados de Lucratividade, Dados de Economia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escopo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limites, Regras, Conteúdos do Projeto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Premissas / Restrições</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O que será necessário para executar o Projeto, O que será restrito no Projeto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Todo o conteúdo a ser desenvolvido no Projeto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagrama de Visão de Negócio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagrama para facilitar o entendimento da Solução.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banco de Dados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabela de Dados dos Sensores, Tabela de Dados dos Clientes, Modelagem Lógica do Projeto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sistema para organizar o desenvolvimento de continuidade do Projeto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VM Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Máquina Virtual Local com Linux para testes, Banco de Dados na VM local.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planilha de Risco do Projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagrama de Solução</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagrama para facilitar o entendimento técnico da Solução.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fluxograma e Ferramenta do Processo de Atendimento do Suporte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolvimento de um fluxograma do processo de atendimento e suporte ao cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cadastro, Login e Dashboard, conectado com BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilizacão da api Data-Viz para validacão e realizacão do login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manual de Instalação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolvimento de um manual para utilizacao de nossa solucão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPT da Apresentação do Projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desenvolvimento da apresentacao para o cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabelas criadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criacao das tabelas necessarias para o projeto no banco de dados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teste Integrado da Solução de IoT (Arduino + Banco de Dados)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilizacao das APIs dat-aqu-ino e data-viz para coleta e exibicao de dados na dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documento de Gestão de Mudanças – GMUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criacão de um padrão de documentacão de gerenciamento de mudancas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IA de apoio ao Suporte N3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integracão do BobIA como ferramenta de suporte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simular cliente-&gt;servidor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distribuir a solução em 2 máquinas. 1 para BD e Aplicação e outra MÁQUINA para coleta de dados do arduino.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projeto EnviroSense - Sprint2 Backlog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projetos atualizado no GitHub / Documentação do Projeto Atualizada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atualização constantes do projetos (Documentação e GitHub)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planilha de Riscos do Projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avalia e mapeia os riscos que o seu projeto pode ter</t>
+    <t>Projeto EnviroSense - Backlog</t>
+  </si>
+  <si>
+    <t>Requisitos</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Classificação</t>
+  </si>
+  <si>
+    <t>Aplicação WEB</t>
+  </si>
+  <si>
+    <t>Tela Inicial, Tela de Login, Tela de Cadastro, Tela de Recuperação de Senha, Simulador Financeiro, Sobre Nós, Dashboard.</t>
+  </si>
+  <si>
+    <t>Essencial.</t>
+  </si>
+  <si>
+    <t>Tela Inicial</t>
+  </si>
+  <si>
+    <t>Título do Projeto, Descrição Sobre o Projeto.</t>
+  </si>
+  <si>
+    <t>Tela de Login</t>
+  </si>
+  <si>
+    <t>Campo de Usuário/E-mail, Campo de Senha, Botão de Visualizar Senha, Botão de Recuperação de Senha, Botão de Login, Botão de Cadastro.</t>
+  </si>
+  <si>
+    <t>Tela de Cadastro</t>
+  </si>
+  <si>
+    <t>Campo de Usuário, Campo de E-mail, Campo de Senha, Campo de Confirmar Senha, Botão de Visualizar Senhas, Botão de Confirmar Cadastro.</t>
+  </si>
+  <si>
+    <t>Tela de Recuperação de Senha</t>
+  </si>
+  <si>
+    <t>Campo de E-mail, Botão de Recuperar Senha, Campo de Confirmação de Código.</t>
+  </si>
+  <si>
+    <t>Simulador Financeiro</t>
+  </si>
+  <si>
+    <t>Aplicação para simular o risco de perdas e multas.</t>
+  </si>
+  <si>
+    <t>Importante.</t>
+  </si>
+  <si>
+    <t>Site Institucional</t>
+  </si>
+  <si>
+    <t>Informações Sobre a Solução, Informações Sobre os Desenvolvedores, Informações Sobre o Segmento.</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Estatísticas, Gráficos, Projeções do dados captados.</t>
+  </si>
+  <si>
+    <t>Documentação</t>
+  </si>
+  <si>
+    <t>Contexto, Objetivo, Justificativa, Escopo, Premissas / Restrições, Requisitos, Diagrama de Visão de Negócio, Protótipo da Aplicação WEB, Projeto Configurado no GitHub.</t>
+  </si>
+  <si>
+    <t>Contexto</t>
+  </si>
+  <si>
+    <t>Explicação do Problema, Explicação do Mercado, Explicação da Solução.</t>
+  </si>
+  <si>
+    <t>Objetivo</t>
+  </si>
+  <si>
+    <t>Pontos a Serem Alcançados.</t>
+  </si>
+  <si>
+    <t>Justificativa</t>
+  </si>
+  <si>
+    <t>Dados de Lucratividade, Dados de Economia.</t>
+  </si>
+  <si>
+    <t>Escopo</t>
+  </si>
+  <si>
+    <t>Limites, Regras, Conteúdos do Projeto.</t>
+  </si>
+  <si>
+    <t>Premissas / Restrições</t>
+  </si>
+  <si>
+    <t>O que será necessário para executar o Projeto, O que será restrito no Projeto.</t>
+  </si>
+  <si>
+    <t>Todo o conteúdo a ser desenvolvido no Projeto.</t>
+  </si>
+  <si>
+    <t>Diagrama de Visão de Negócio</t>
+  </si>
+  <si>
+    <t>Diagrama para facilitar o entendimento da Solução.</t>
+  </si>
+  <si>
+    <t>Banco de Dados</t>
+  </si>
+  <si>
+    <t>Tabela de Dados dos Sensores, Tabela de Dados dos Clientes, Modelagem Lógica do Projeto.</t>
+  </si>
+  <si>
+    <t>Trello</t>
+  </si>
+  <si>
+    <t>Sistema para organizar o desenvolvimento de continuidade do Projeto.</t>
+  </si>
+  <si>
+    <t>VM Local</t>
+  </si>
+  <si>
+    <t>Máquina Virtual Local com Linux para testes, Banco de Dados na VM local.</t>
+  </si>
+  <si>
+    <t>Planilha de Risco do Projeto</t>
+  </si>
+  <si>
+    <t>Diagrama de Solução</t>
+  </si>
+  <si>
+    <t>Diagrama para facilitar o entendimento técnico da Solução.</t>
+  </si>
+  <si>
+    <t>Fluxograma e Ferramenta do Processo de Atendimento do Suporte</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de um fluxograma do processo de atendimento e suporte ao cliente</t>
+  </si>
+  <si>
+    <t>Cadastro, Login e Dashboard, conectado com BD</t>
+  </si>
+  <si>
+    <t>Utilizacão da api Data-Viz para validacão e realizacão do login</t>
+  </si>
+  <si>
+    <t>Manual de Instalação</t>
+  </si>
+  <si>
+    <t>Desenvolvimento de um manual para utilizacao de nossa solucão</t>
+  </si>
+  <si>
+    <t>PPT da Apresentação do Projeto</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da apresentacao para o cliente</t>
+  </si>
+  <si>
+    <t>Tabelas criadas</t>
+  </si>
+  <si>
+    <t>Criacao das tabelas necessarias para o projeto no banco de dados</t>
+  </si>
+  <si>
+    <t>Teste Integrado da Solução de IoT (Arduino + Banco de Dados)</t>
+  </si>
+  <si>
+    <t>Utilizacao das APIs dat-aqu-ino e data-viz para coleta e exibicao de dados na dashboard</t>
+  </si>
+  <si>
+    <t>Documento de Gestão de Mudanças – GMUD</t>
+  </si>
+  <si>
+    <t>Criacão de um padrão de documentacão de gerenciamento de mudancas</t>
+  </si>
+  <si>
+    <t>IA de apoio ao Suporte N3</t>
+  </si>
+  <si>
+    <t>Integracão do BobIA como ferramenta de suporte</t>
+  </si>
+  <si>
+    <t>Simular cliente-&gt;servidor.</t>
+  </si>
+  <si>
+    <t>Distribuir a solução em 2 máquinas. 1 para BD e Aplicação e outra MÁQUINA para coleta de dados do arduino.</t>
+  </si>
+  <si>
+    <t>Projeto EnviroSense - Sprint2 Backlog</t>
+  </si>
+  <si>
+    <t>Projetos atualizado no GitHub / Documentação do Projeto Atualizada</t>
+  </si>
+  <si>
+    <t>Atualização constantes do projetos (Documentação e GitHub)</t>
+  </si>
+  <si>
+    <t>Planilha de Riscos do Projeto</t>
+  </si>
+  <si>
+    <t>Avalia e mapeia os riscos que o seu projeto pode ter</t>
   </si>
   <si>
     <t xml:space="preserve"> Especificação da Dashboard</t>
   </si>
   <si>
-    <t xml:space="preserve">Quais tipos de dados aparecerão na Dashboard</t>
+    <t>Quais tipos de dados aparecerão na Dashboard</t>
   </si>
   <si>
     <t xml:space="preserve"> Site Estático Institucional – Local em HTML/CSS/JavaScript</t>
   </si>
   <si>
-    <t xml:space="preserve">Criação do site estático institucional da empresa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site Estático Dashboard (Gráfico com ChartJS) - Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criação do site com as dashboards contendo dados do sensor</t>
+    <t>Criação do site estático institucional da empresa</t>
+  </si>
+  <si>
+    <t>Site Estático Dashboard (Gráfico com ChartJS) - Local</t>
+  </si>
+  <si>
+    <t>Criação do site com as dashboards contendo dados do sensor</t>
   </si>
   <si>
     <t xml:space="preserve"> Site Estático Cadastro e Login – Local ( com conceito de repetições)</t>
   </si>
   <si>
-    <t xml:space="preserve">Criação do site com tela de cadastro e login para o cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagrama de Solução (Arquitetura Técnica do Projeto)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagrama mostrando a solução técnica do seu projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atividades organizadas na ferramenta de Gestão (Sprints / Atividades)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organização das tarefas do time de acordo com a sprint</t>
+    <t>Criação do site com tela de cadastro e login para o cliente</t>
+  </si>
+  <si>
+    <t>Diagrama de Solução (Arquitetura Técnica do Projeto)</t>
+  </si>
+  <si>
+    <t>Diagrama mostrando a solução técnica do seu projeto</t>
+  </si>
+  <si>
+    <t>Atividades organizadas na ferramenta de Gestão (Sprints / Atividades)</t>
+  </si>
+  <si>
+    <t>Organização das tarefas do time de acordo com a sprint</t>
   </si>
   <si>
     <t xml:space="preserve"> BackLog da Sprint (Demanda, Pontuação, Prioridade)</t>
   </si>
   <si>
-    <t xml:space="preserve">Levantamento de requisitos pertinentes à Sprint atual</t>
+    <t>Levantamento de requisitos pertinentes à Sprint atual</t>
   </si>
   <si>
     <t xml:space="preserve"> Modelagem Lógica do Projeto v1</t>
   </si>
   <si>
-    <t xml:space="preserve">Modelagem de relacionamento entre as tabelas do BD</t>
+    <t>Modelagem de relacionamento entre as tabelas do BD</t>
   </si>
   <si>
     <t xml:space="preserve"> Script de criação do Banco / Tabelas criadas em BD local</t>
   </si>
   <si>
-    <t xml:space="preserve">Criação das tabelas e scripts</t>
+    <t>Criação das tabelas e scripts</t>
   </si>
   <si>
     <t xml:space="preserve"> Simular a integração do Sistema ( utilização do Sensor + Gráfico )</t>
   </si>
   <si>
-    <t xml:space="preserve">Integração do sistema ao sensor de gás</t>
+    <t>Integração do sistema ao sensor de gás</t>
   </si>
   <si>
     <t xml:space="preserve"> Usar API Local / Sensor</t>
   </si>
   <si>
-    <t xml:space="preserve">Utilização da API para captação de dados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalar MYSQL na VMLinux e inserção de dados do Arduíno no MySQL na mesma máquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalação do SGBD na VM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validar a solução técnica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validação do diagrama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projeto EnviroSense – Sprint3 Backlog</t>
+    <t>Utilização da API para captação de dados</t>
+  </si>
+  <si>
+    <t>Instalar MYSQL na VMLinux e inserção de dados do Arduíno no MySQL na mesma máquina</t>
+  </si>
+  <si>
+    <t>Instalação do SGBD na VM</t>
+  </si>
+  <si>
+    <t>Validar a solução técnica</t>
+  </si>
+  <si>
+    <t>Validação do diagrama</t>
+  </si>
+  <si>
+    <t>Projeto EnviroSense – Sprint3 Backlog</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -328,41 +330,23 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -386,89 +370,107 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="4">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4EA72E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF0D0D0D"/>
       </font>
@@ -480,7 +482,19 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4EA72E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF000000"/>
       </font>
@@ -492,7 +506,19 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0D0D0D"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color rgb="FF000000"/>
       </font>
@@ -504,19 +530,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color rgb="FF0D0D0D"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
         <color rgb="FF000000"/>
       </font>
@@ -528,17 +542,18 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
-        <color rgb="FF000000"/>
+        <color rgb="FF0D0D0D"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF4EA72E"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -597,30 +612,358 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="174.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.85"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1"/>
+    <col min="3" max="3" width="174.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="2:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +971,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -639,7 +982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -650,7 +993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
@@ -661,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -672,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -683,7 +1026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -694,7 +1037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -705,7 +1048,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
@@ -716,7 +1059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
@@ -727,7 +1070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
@@ -738,7 +1081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
@@ -749,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
@@ -760,7 +1103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
@@ -771,7 +1114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
@@ -782,7 +1125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
@@ -793,7 +1136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>1</v>
       </c>
@@ -804,7 +1147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
@@ -815,7 +1158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>37</v>
       </c>
@@ -826,7 +1169,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>39</v>
       </c>
@@ -837,7 +1180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>41</v>
       </c>
@@ -848,7 +1191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
@@ -857,7 +1200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>44</v>
       </c>
@@ -868,7 +1211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>46</v>
       </c>
@@ -879,7 +1222,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
@@ -890,7 +1233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>50</v>
       </c>
@@ -901,8 +1244,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="5" t="s">
@@ -912,8 +1255,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -923,8 +1266,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -934,8 +1277,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="5" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -945,7 +1288,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>60</v>
       </c>
@@ -956,7 +1299,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>62</v>
       </c>
@@ -971,72 +1314,45 @@
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3:D23 D49:D1048576">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+  <conditionalFormatting sqref="D3:D32 D49:D1048576">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Importante."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D23 D49:D1048576">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Essencial."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D23 D49:D1048576">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Desejável."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D32">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>"Importante."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D32">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>"Essencial."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24:D32">
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>"Desejável."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555556" right="0.511805555555556" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="77.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.49"/>
+    <col min="1" max="1" width="77.140625" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1047,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>65</v>
       </c>
@@ -1058,7 +1374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>67</v>
       </c>
@@ -1069,7 +1385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>69</v>
       </c>
@@ -1080,7 +1396,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>71</v>
       </c>
@@ -1091,7 +1407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>73</v>
       </c>
@@ -1102,7 +1418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>75</v>
       </c>
@@ -1113,7 +1429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>77</v>
       </c>
@@ -1124,7 +1440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -1135,7 +1451,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
@@ -1146,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -1157,7 +1473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>85</v>
       </c>
@@ -1168,7 +1484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>87</v>
       </c>
@@ -1179,7 +1495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>89</v>
       </c>
@@ -1190,7 +1506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>91</v>
       </c>
@@ -1201,7 +1517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>93</v>
       </c>
@@ -1212,30 +1528,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C17">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"Importante."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C17">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Essencial."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C17">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Desejável."</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
   </headerFooter>
@@ -1243,31 +1553,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="115.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.85"/>
+    <col min="1" max="1" width="115.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1278,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -1289,7 +1596,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>48</v>
       </c>
@@ -1300,7 +1607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>50</v>
       </c>
@@ -1311,7 +1618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>52</v>
       </c>
@@ -1322,8 +1629,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1333,8 +1640,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1344,7 +1651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>58</v>
       </c>
@@ -1355,7 +1662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>60</v>
       </c>
@@ -1366,7 +1673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
@@ -1377,38 +1684,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C11">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Importante."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C11">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Essencial."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C11">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Desejável."</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>